<commit_message>
cleaned commands, and minor condition
</commit_message>
<xml_diff>
--- a/public/uploads/Test_Sample_v3.xlsx
+++ b/public/uploads/Test_Sample_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haridher\Downloads\archived_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2AC450-6F2A-4A49-909E-1A61EE9A1C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C33441-0DCB-41F8-A125-4CE296980BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{330C708C-5D41-460D-8AE7-4DC33D46AD04}"/>
   </bookViews>
@@ -5789,7 +5789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5105C0CE-81ED-4EAC-85F2-91D87B6ED407}">
   <dimension ref="A1:BA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>